<commit_message>
made some addtions to text translation
</commit_message>
<xml_diff>
--- a/text_translation.xlsx
+++ b/text_translation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nique\Music\faber_compendiolum_musicae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8B18F6-2701-451E-A5D0-5593170BA391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7EC5CF-065B-4DC7-8E7C-CFB1173EDD91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D007FBED-DCD4-47CB-95B1-EB83ED864BB1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Da regulas de notis simplicibus</t>
   </si>
@@ -128,6 +128,117 @@
   </si>
   <si>
     <t>http://www.chmtl.indiana.edu/tml/16th/FABCOM_TEXT.html</t>
+  </si>
+  <si>
+    <t>Quid est Musica?</t>
+  </si>
+  <si>
+    <t>Est bene canendi scientia.</t>
+  </si>
+  <si>
+    <t>Quotuplex est?</t>
+  </si>
+  <si>
+    <t>Quid est Musica Choralis?</t>
+  </si>
+  <si>
+    <t>Quae simplicem et uniformem in suis notulis servat mensuram.</t>
+  </si>
+  <si>
+    <t>Quid est Musica Figuralis?</t>
+  </si>
+  <si>
+    <t>Quae diversam figurarum quantitatem, juxta varia praescripta signa exprimit.</t>
+  </si>
+  <si>
+    <t>Quot sunt praecipua capita, quibus tyro opus habet?</t>
+  </si>
+  <si>
+    <t>pg 8</t>
+  </si>
+  <si>
+    <t>What is music?</t>
+  </si>
+  <si>
+    <t>Sie iſt ein kunſtrecht vnd wohl zu ſingen</t>
+  </si>
+  <si>
+    <t>It is a well sung science / It is a good thing to sing.</t>
+  </si>
+  <si>
+    <t>Wievilfaltig iſt ſie</t>
+  </si>
+  <si>
+    <t>How many is it? / How diverse is it? / How varied is it?</t>
+  </si>
+  <si>
+    <t>Duplex -&gt; Choralis est Figuralis</t>
+  </si>
+  <si>
+    <t>Zwifaltig. Choralis oder gleichförmig/ und Figuralis oder vilförmlich.</t>
+  </si>
+  <si>
+    <t>Double -&gt; Choral and Figured</t>
+  </si>
+  <si>
+    <t>What is Choral Music</t>
+  </si>
+  <si>
+    <t>What is musica figuralis?</t>
+  </si>
+  <si>
+    <t>Welche ein einfachen vnnd gleichförmigen Tact oder Menſur in jren Noten haltet.</t>
+  </si>
+  <si>
+    <t>That which is simple and uniform, keeps notes in their measure | Simple and uniform tact or mensur in your notes</t>
+  </si>
+  <si>
+    <t>That which requires a different quantity of figures, according to the prescriptions of the standards of a variety of sounds. | That which has uneven sizes of notes and pauses</t>
+  </si>
+  <si>
+    <t>Welche ein ungleiche gröſſe der Noten und Pauſen hat - nach mancherlen fürgeſetzten zeichen.</t>
+  </si>
+  <si>
+    <t>What are the most important notes that the beginner needs?</t>
+  </si>
+  <si>
+    <t> Quinque, Clavis, Vox, Cantus, Mutatio et Figura</t>
+  </si>
+  <si>
+    <t>pg9</t>
+  </si>
+  <si>
+    <t>Quid est clavis?</t>
+  </si>
+  <si>
+    <t>Est vocis formandae index.</t>
+  </si>
+  <si>
+    <t>Quot sunt claves?</t>
+  </si>
+  <si>
+    <t>Viginti. Atque ex sequenti figura, quae vulgo Scala dicitur, patent.</t>
+  </si>
+  <si>
+    <t>What is the Clavis?</t>
+  </si>
+  <si>
+    <t>Five: Clavis (Music Key), voice, singing, mutation, and figure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is the voice to be formed index; It is the pointer to the voice that you want to sing. </t>
+  </si>
+  <si>
+    <t>wieviel sind musikschlüssel</t>
+  </si>
+  <si>
+    <t>How are the musical keys?</t>
+  </si>
+  <si>
+    <t>20. Now from the following figure, which is commonly known as the scale</t>
+  </si>
+  <si>
+    <t>Zweinzig und werden außnachfolgenden Täfelein ertände das gemeiniglich Scala (ein Leiter) genennet wird.</t>
   </si>
 </sst>
 </file>
@@ -493,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91971CD0-FCDD-40D9-8B47-7068D9385128}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -521,115 +632,258 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>